<commit_message>
Added clusters to projects
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="d8JdM1G91/1GS+kNXhlyzui+1+JyDp7qXMX0PW1XctA="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -149,13 +154,52 @@
   </si>
   <si>
     <t>HCFCIND</t>
+  </si>
+  <si>
+    <t>Energy Eficiency</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Disposal</t>
+  </si>
+  <si>
+    <t>CFC Individual</t>
+  </si>
+  <si>
+    <t>CFCIND</t>
+  </si>
+  <si>
+    <t>CFC Phase-out Plans</t>
+  </si>
+  <si>
+    <t>CPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Sector Plans</t>
+  </si>
+  <si>
+    <t>OOSP</t>
+  </si>
+  <si>
+    <t>CFC Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>CPPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>OOPPP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -185,6 +229,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -201,64 +250,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -273,135 +266,49 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -632,47 +539,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -681,13 +588,13 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -696,213 +603,213 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="11"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="11"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -911,617 +818,665 @@
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="25"/>
+      <c r="A22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="25"/>
+      <c r="A23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="25"/>
+      <c r="A24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="25"/>
+      <c r="A25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="25"/>
+      <c r="A26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="25"/>
+      <c r="A27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="25"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="25"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="25"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="25"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="25"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="25"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="25"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="25"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="25"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="25"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="25"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="25"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="25"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="25"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="25"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="25"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="25"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="25"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="25"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="25"/>
+      <c r="C47" s="15"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="25"/>
+      <c r="C48" s="15"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="25"/>
+      <c r="C49" s="15"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="25"/>
+      <c r="C50" s="15"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="25"/>
+      <c r="C51" s="15"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="25"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="25"/>
+      <c r="C53" s="15"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="25"/>
+      <c r="C54" s="15"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="25"/>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="25"/>
+      <c r="C56" s="15"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="25"/>
+      <c r="C57" s="15"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="25"/>
+      <c r="C58" s="15"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="25"/>
+      <c r="C59" s="15"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="25"/>
+      <c r="C60" s="15"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="25"/>
+      <c r="C61" s="15"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="25"/>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="25"/>
+      <c r="C63" s="15"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="25"/>
+      <c r="C64" s="15"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="25"/>
+      <c r="C65" s="15"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="25"/>
+      <c r="C66" s="15"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="25"/>
+      <c r="C67" s="15"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="25"/>
+      <c r="C68" s="15"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="25"/>
+      <c r="C69" s="15"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="25"/>
+      <c r="C70" s="15"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="25"/>
+      <c r="C71" s="15"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="25"/>
+      <c r="C72" s="15"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="25"/>
+      <c r="C73" s="15"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="25"/>
+      <c r="C74" s="15"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="25"/>
+      <c r="C75" s="15"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="25"/>
+      <c r="C76" s="15"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="25"/>
+      <c r="C77" s="15"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="25"/>
+      <c r="C78" s="15"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="25"/>
+      <c r="C79" s="15"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="25"/>
+      <c r="C80" s="15"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="25"/>
+      <c r="C81" s="15"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="25"/>
+      <c r="C82" s="15"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="25"/>
+      <c r="C83" s="15"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="25"/>
+      <c r="C84" s="15"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="25"/>
+      <c r="C85" s="15"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="25"/>
+      <c r="C86" s="15"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="25"/>
+      <c r="C87" s="15"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="25"/>
+      <c r="C88" s="15"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="25"/>
+      <c r="C89" s="15"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="25"/>
+      <c r="C90" s="15"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="25"/>
+      <c r="C91" s="15"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="25"/>
+      <c r="C92" s="15"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="25"/>
+      <c r="C93" s="15"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="25"/>
+      <c r="C94" s="15"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="25"/>
+      <c r="C95" s="15"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="25"/>
+      <c r="C96" s="15"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="25"/>
+      <c r="C97" s="15"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="25"/>
+      <c r="C98" s="15"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="25"/>
+      <c r="C99" s="15"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="25"/>
+      <c r="C100" s="15"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="25"/>
+      <c r="C101" s="15"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="25"/>
+      <c r="C102" s="15"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="25"/>
+      <c r="C103" s="15"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="25"/>
+      <c r="C104" s="15"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="25"/>
+      <c r="C105" s="15"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="25"/>
+      <c r="C106" s="15"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="25"/>
+      <c r="C107" s="15"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="25"/>
+      <c r="C108" s="15"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="25"/>
+      <c r="C109" s="15"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="25"/>
+      <c r="C110" s="15"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="25"/>
+      <c r="C111" s="15"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="25"/>
+      <c r="C112" s="15"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="25"/>
+      <c r="C113" s="15"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="25"/>
+      <c r="C114" s="15"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="25"/>
+      <c r="C115" s="15"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="25"/>
+      <c r="C116" s="15"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="25"/>
+      <c r="C117" s="15"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="25"/>
+      <c r="C118" s="15"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="25"/>
+      <c r="C119" s="15"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="25"/>
+      <c r="C120" s="15"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="25"/>
+      <c r="C121" s="15"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="25"/>
+      <c r="C122" s="15"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="25"/>
+      <c r="C123" s="15"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="25"/>
+      <c r="C124" s="15"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="25"/>
+      <c r="C125" s="15"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="25"/>
+      <c r="C126" s="15"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="25"/>
+      <c r="C127" s="15"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="25"/>
+      <c r="C128" s="15"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="25"/>
+      <c r="C129" s="15"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="25"/>
+      <c r="C130" s="15"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="25"/>
+      <c r="C131" s="15"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="25"/>
+      <c r="C132" s="15"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="25"/>
+      <c r="C133" s="15"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="25"/>
+      <c r="C134" s="15"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="25"/>
+      <c r="C135" s="15"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="25"/>
+      <c r="C136" s="15"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="25"/>
+      <c r="C137" s="15"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="25"/>
+      <c r="C138" s="15"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="25"/>
+      <c r="C139" s="15"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="25"/>
+      <c r="C140" s="15"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="25"/>
+      <c r="C141" s="15"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="25"/>
+      <c r="C142" s="15"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="25"/>
+      <c r="C143" s="15"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="25"/>
+      <c r="C144" s="15"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="25"/>
+      <c r="C145" s="15"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="25"/>
+      <c r="C146" s="15"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="25"/>
+      <c r="C147" s="15"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="25"/>
+      <c r="C148" s="15"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="25"/>
+      <c r="C149" s="15"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="25"/>
+      <c r="C150" s="15"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="25"/>
+      <c r="C151" s="15"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="25"/>
+      <c r="C152" s="15"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="25"/>
+      <c r="C153" s="15"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="25"/>
+      <c r="C154" s="15"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="25"/>
+      <c r="C155" s="15"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="25"/>
+      <c r="C156" s="15"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="25"/>
+      <c r="C157" s="15"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="25"/>
+      <c r="C158" s="15"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="25"/>
+      <c r="C159" s="15"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="25"/>
+      <c r="C160" s="15"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="25"/>
+      <c r="C161" s="15"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="25"/>
+      <c r="C162" s="15"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="25"/>
+      <c r="C163" s="15"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="25"/>
+      <c r="C164" s="15"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="25"/>
+      <c r="C165" s="15"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="25"/>
+      <c r="C166" s="15"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="25"/>
+      <c r="C167" s="15"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="25"/>
+      <c r="C168" s="15"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="25"/>
+      <c r="C169" s="15"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="25"/>
+      <c r="C170" s="15"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="25"/>
+      <c r="C171" s="15"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="25"/>
+      <c r="C172" s="15"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="25"/>
+      <c r="C173" s="15"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="25"/>
+      <c r="C174" s="15"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="25"/>
+      <c r="C175" s="15"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="25"/>
+      <c r="C176" s="15"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="25"/>
+      <c r="C177" s="15"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="25"/>
+      <c r="C178" s="15"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="25"/>
+      <c r="C179" s="15"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="25"/>
+      <c r="C180" s="15"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="25"/>
+      <c r="C181" s="15"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="25"/>
+      <c r="C182" s="15"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="25"/>
+      <c r="C183" s="15"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="25"/>
+      <c r="C184" s="15"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="25"/>
+      <c r="C185" s="15"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="25"/>
+      <c r="C186" s="15"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="25"/>
+      <c r="C187" s="15"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="25"/>
+      <c r="C188" s="15"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="25"/>
+      <c r="C189" s="15"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="25"/>
+      <c r="C190" s="15"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="25"/>
+      <c r="C191" s="15"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="25"/>
+      <c r="C192" s="15"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="25"/>
+      <c r="C193" s="15"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="25"/>
+      <c r="C194" s="15"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="25"/>
+      <c r="C195" s="15"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="25"/>
+      <c r="C196" s="15"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="25"/>
+      <c r="C197" s="15"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="25"/>
+      <c r="C198" s="15"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="25"/>
+      <c r="C199" s="15"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="25"/>
+      <c r="C200" s="15"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="25"/>
+      <c r="C201" s="15"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="25"/>
+      <c r="C202" s="15"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="25"/>
+      <c r="C203" s="15"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="25"/>
+      <c r="C204" s="15"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="25"/>
+      <c r="C205" s="15"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="25"/>
+      <c r="C206" s="15"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="25"/>
+      <c r="C207" s="15"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="25"/>
+      <c r="C208" s="15"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="25"/>
+      <c r="C209" s="15"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="25"/>
+      <c r="C210" s="15"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="25"/>
+      <c r="C211" s="15"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="25"/>
+      <c r="C212" s="15"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="25"/>
+      <c r="C213" s="15"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="25"/>
+      <c r="C214" s="15"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="25"/>
+      <c r="C215" s="15"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="25"/>
+      <c r="C216" s="15"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="25"/>
+      <c r="C217" s="15"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="25"/>
+      <c r="C218" s="15"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="25"/>
+      <c r="C219" s="15"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="25"/>
-    </row>
-    <row r="221" ht="15.75" customHeight="1">
-      <c r="C221" s="25"/>
-    </row>
+      <c r="C220" s="15"/>
+    </row>
+    <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
     <row r="223" ht="15.75" customHeight="1"/>
     <row r="224" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
New code generator (#135)
* Generated meta projects code

* Generated  project sub codes

* Updated sector/subsector mapping list

* Added clusters to projects

* Fixed mini bug

* Mini update
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="d8JdM1G91/1GS+kNXhlyzui+1+JyDp7qXMX0PW1XctA="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -149,13 +154,52 @@
   </si>
   <si>
     <t>HCFCIND</t>
+  </si>
+  <si>
+    <t>Energy Eficiency</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Disposal</t>
+  </si>
+  <si>
+    <t>CFC Individual</t>
+  </si>
+  <si>
+    <t>CFCIND</t>
+  </si>
+  <si>
+    <t>CFC Phase-out Plans</t>
+  </si>
+  <si>
+    <t>CPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Sector Plans</t>
+  </si>
+  <si>
+    <t>OOSP</t>
+  </si>
+  <si>
+    <t>CFC Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>CPPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>OOPPP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -185,6 +229,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -201,64 +250,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -273,135 +266,49 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -632,47 +539,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -681,13 +588,13 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -696,213 +603,213 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="11"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="11"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -911,617 +818,665 @@
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="25"/>
+      <c r="A22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="25"/>
+      <c r="A23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="25"/>
+      <c r="A24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="25"/>
+      <c r="A25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="25"/>
+      <c r="A26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="25"/>
+      <c r="A27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="25"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="25"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="25"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="25"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="25"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="25"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="25"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="25"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="25"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="25"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="25"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="25"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="25"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="25"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="25"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="25"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="25"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="25"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="25"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="25"/>
+      <c r="C47" s="15"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="25"/>
+      <c r="C48" s="15"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="25"/>
+      <c r="C49" s="15"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="25"/>
+      <c r="C50" s="15"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="25"/>
+      <c r="C51" s="15"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="25"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="25"/>
+      <c r="C53" s="15"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="25"/>
+      <c r="C54" s="15"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="25"/>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="25"/>
+      <c r="C56" s="15"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="25"/>
+      <c r="C57" s="15"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="25"/>
+      <c r="C58" s="15"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="25"/>
+      <c r="C59" s="15"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="25"/>
+      <c r="C60" s="15"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="25"/>
+      <c r="C61" s="15"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="25"/>
+      <c r="C62" s="15"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="25"/>
+      <c r="C63" s="15"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="25"/>
+      <c r="C64" s="15"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="25"/>
+      <c r="C65" s="15"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="25"/>
+      <c r="C66" s="15"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="25"/>
+      <c r="C67" s="15"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="25"/>
+      <c r="C68" s="15"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="25"/>
+      <c r="C69" s="15"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="25"/>
+      <c r="C70" s="15"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="25"/>
+      <c r="C71" s="15"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="25"/>
+      <c r="C72" s="15"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="25"/>
+      <c r="C73" s="15"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="25"/>
+      <c r="C74" s="15"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="25"/>
+      <c r="C75" s="15"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="25"/>
+      <c r="C76" s="15"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="25"/>
+      <c r="C77" s="15"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="25"/>
+      <c r="C78" s="15"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="25"/>
+      <c r="C79" s="15"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="25"/>
+      <c r="C80" s="15"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="25"/>
+      <c r="C81" s="15"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="25"/>
+      <c r="C82" s="15"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="25"/>
+      <c r="C83" s="15"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="25"/>
+      <c r="C84" s="15"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="25"/>
+      <c r="C85" s="15"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="25"/>
+      <c r="C86" s="15"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="25"/>
+      <c r="C87" s="15"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="25"/>
+      <c r="C88" s="15"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="25"/>
+      <c r="C89" s="15"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="25"/>
+      <c r="C90" s="15"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="25"/>
+      <c r="C91" s="15"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="25"/>
+      <c r="C92" s="15"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="25"/>
+      <c r="C93" s="15"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="25"/>
+      <c r="C94" s="15"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="25"/>
+      <c r="C95" s="15"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="25"/>
+      <c r="C96" s="15"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="25"/>
+      <c r="C97" s="15"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="25"/>
+      <c r="C98" s="15"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="25"/>
+      <c r="C99" s="15"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="25"/>
+      <c r="C100" s="15"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="25"/>
+      <c r="C101" s="15"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="25"/>
+      <c r="C102" s="15"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="25"/>
+      <c r="C103" s="15"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="25"/>
+      <c r="C104" s="15"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="25"/>
+      <c r="C105" s="15"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="25"/>
+      <c r="C106" s="15"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="25"/>
+      <c r="C107" s="15"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="25"/>
+      <c r="C108" s="15"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="25"/>
+      <c r="C109" s="15"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="25"/>
+      <c r="C110" s="15"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="25"/>
+      <c r="C111" s="15"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="25"/>
+      <c r="C112" s="15"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="25"/>
+      <c r="C113" s="15"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="25"/>
+      <c r="C114" s="15"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="25"/>
+      <c r="C115" s="15"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="25"/>
+      <c r="C116" s="15"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="25"/>
+      <c r="C117" s="15"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="25"/>
+      <c r="C118" s="15"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="25"/>
+      <c r="C119" s="15"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="25"/>
+      <c r="C120" s="15"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="25"/>
+      <c r="C121" s="15"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="25"/>
+      <c r="C122" s="15"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="25"/>
+      <c r="C123" s="15"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="25"/>
+      <c r="C124" s="15"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="25"/>
+      <c r="C125" s="15"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="25"/>
+      <c r="C126" s="15"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="25"/>
+      <c r="C127" s="15"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="25"/>
+      <c r="C128" s="15"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="25"/>
+      <c r="C129" s="15"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="25"/>
+      <c r="C130" s="15"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="25"/>
+      <c r="C131" s="15"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="25"/>
+      <c r="C132" s="15"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="25"/>
+      <c r="C133" s="15"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="25"/>
+      <c r="C134" s="15"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="25"/>
+      <c r="C135" s="15"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="25"/>
+      <c r="C136" s="15"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="25"/>
+      <c r="C137" s="15"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="25"/>
+      <c r="C138" s="15"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="25"/>
+      <c r="C139" s="15"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="25"/>
+      <c r="C140" s="15"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="25"/>
+      <c r="C141" s="15"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="25"/>
+      <c r="C142" s="15"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="25"/>
+      <c r="C143" s="15"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="25"/>
+      <c r="C144" s="15"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="25"/>
+      <c r="C145" s="15"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="25"/>
+      <c r="C146" s="15"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="25"/>
+      <c r="C147" s="15"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="25"/>
+      <c r="C148" s="15"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="25"/>
+      <c r="C149" s="15"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="25"/>
+      <c r="C150" s="15"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="25"/>
+      <c r="C151" s="15"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="25"/>
+      <c r="C152" s="15"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="25"/>
+      <c r="C153" s="15"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="25"/>
+      <c r="C154" s="15"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="25"/>
+      <c r="C155" s="15"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="25"/>
+      <c r="C156" s="15"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="25"/>
+      <c r="C157" s="15"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="25"/>
+      <c r="C158" s="15"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="25"/>
+      <c r="C159" s="15"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="25"/>
+      <c r="C160" s="15"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="25"/>
+      <c r="C161" s="15"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="25"/>
+      <c r="C162" s="15"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="25"/>
+      <c r="C163" s="15"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="25"/>
+      <c r="C164" s="15"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="25"/>
+      <c r="C165" s="15"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="25"/>
+      <c r="C166" s="15"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="25"/>
+      <c r="C167" s="15"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="25"/>
+      <c r="C168" s="15"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="25"/>
+      <c r="C169" s="15"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="25"/>
+      <c r="C170" s="15"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="25"/>
+      <c r="C171" s="15"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="25"/>
+      <c r="C172" s="15"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="25"/>
+      <c r="C173" s="15"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="25"/>
+      <c r="C174" s="15"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="25"/>
+      <c r="C175" s="15"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="25"/>
+      <c r="C176" s="15"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="25"/>
+      <c r="C177" s="15"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="25"/>
+      <c r="C178" s="15"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="25"/>
+      <c r="C179" s="15"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="25"/>
+      <c r="C180" s="15"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="25"/>
+      <c r="C181" s="15"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="25"/>
+      <c r="C182" s="15"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="25"/>
+      <c r="C183" s="15"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="25"/>
+      <c r="C184" s="15"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="25"/>
+      <c r="C185" s="15"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="25"/>
+      <c r="C186" s="15"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="25"/>
+      <c r="C187" s="15"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="25"/>
+      <c r="C188" s="15"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="25"/>
+      <c r="C189" s="15"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="25"/>
+      <c r="C190" s="15"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="25"/>
+      <c r="C191" s="15"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="25"/>
+      <c r="C192" s="15"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="25"/>
+      <c r="C193" s="15"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="25"/>
+      <c r="C194" s="15"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="25"/>
+      <c r="C195" s="15"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="25"/>
+      <c r="C196" s="15"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="25"/>
+      <c r="C197" s="15"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="25"/>
+      <c r="C198" s="15"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="25"/>
+      <c r="C199" s="15"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="25"/>
+      <c r="C200" s="15"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="25"/>
+      <c r="C201" s="15"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="25"/>
+      <c r="C202" s="15"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="25"/>
+      <c r="C203" s="15"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="25"/>
+      <c r="C204" s="15"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="25"/>
+      <c r="C205" s="15"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="25"/>
+      <c r="C206" s="15"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="25"/>
+      <c r="C207" s="15"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="25"/>
+      <c r="C208" s="15"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="25"/>
+      <c r="C209" s="15"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="25"/>
+      <c r="C210" s="15"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="25"/>
+      <c r="C211" s="15"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="25"/>
+      <c r="C212" s="15"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="25"/>
+      <c r="C213" s="15"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="25"/>
+      <c r="C214" s="15"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="25"/>
+      <c r="C215" s="15"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="25"/>
+      <c r="C216" s="15"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="25"/>
+      <c r="C217" s="15"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="25"/>
+      <c r="C218" s="15"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="25"/>
+      <c r="C219" s="15"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="25"/>
-    </row>
-    <row r="221" ht="15.75" customHeight="1">
-      <c r="C221" s="25"/>
-    </row>
+      <c r="C220" s="15"/>
+    </row>
+    <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
     <row r="223" ht="15.75" customHeight="1"/>
     <row r="224" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added regions and subregions in country
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -193,13 +193,25 @@
   </si>
   <si>
     <t>OOPPP</t>
+  </si>
+  <si>
+    <t>Technical assistance</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>TRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -212,22 +224,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF274180"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -250,65 +253,39 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -545,29 +522,29 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -576,10 +553,10 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -591,10 +568,10 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -606,109 +583,109 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
@@ -723,8 +700,8 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -736,69 +713,69 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -807,9 +784,9 @@
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -818,663 +795,679 @@
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="15"/>
+      <c r="A28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="15"/>
+      <c r="A29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="15"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="15"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="15"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="15"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="15"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="15"/>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="15"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="15"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="15"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="15"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="15"/>
+      <c r="C40" s="11"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="15"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="15"/>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="15"/>
+      <c r="C43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="15"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="15"/>
+      <c r="C45" s="11"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="15"/>
+      <c r="C46" s="11"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="15"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="15"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="15"/>
+      <c r="C49" s="11"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="15"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="15"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="15"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="15"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="15"/>
+      <c r="C54" s="11"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="15"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="15"/>
+      <c r="C56" s="11"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="15"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="15"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="15"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="15"/>
+      <c r="C60" s="11"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="15"/>
+      <c r="C61" s="11"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="15"/>
+      <c r="C62" s="11"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="15"/>
+      <c r="C63" s="11"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="15"/>
+      <c r="C64" s="11"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="15"/>
+      <c r="C65" s="11"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="15"/>
+      <c r="C66" s="11"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="15"/>
+      <c r="C67" s="11"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="15"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="15"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="15"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="15"/>
+      <c r="C71" s="11"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="15"/>
+      <c r="C72" s="11"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="15"/>
+      <c r="C73" s="11"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="15"/>
+      <c r="C74" s="11"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="15"/>
+      <c r="C75" s="11"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="15"/>
+      <c r="C76" s="11"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="15"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="15"/>
+      <c r="C78" s="11"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="15"/>
+      <c r="C79" s="11"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="15"/>
+      <c r="C80" s="11"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="15"/>
+      <c r="C81" s="11"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="15"/>
+      <c r="C82" s="11"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="15"/>
+      <c r="C83" s="11"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="15"/>
+      <c r="C84" s="11"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="15"/>
+      <c r="C85" s="11"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="15"/>
+      <c r="C86" s="11"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="15"/>
+      <c r="C87" s="11"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="15"/>
+      <c r="C88" s="11"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="15"/>
+      <c r="C89" s="11"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="15"/>
+      <c r="C90" s="11"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="15"/>
+      <c r="C91" s="11"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="15"/>
+      <c r="C92" s="11"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="15"/>
+      <c r="C93" s="11"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="15"/>
+      <c r="C94" s="11"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="15"/>
+      <c r="C95" s="11"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="15"/>
+      <c r="C96" s="11"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="15"/>
+      <c r="C97" s="11"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="15"/>
+      <c r="C98" s="11"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="15"/>
+      <c r="C99" s="11"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="15"/>
+      <c r="C100" s="11"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="15"/>
+      <c r="C101" s="11"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="15"/>
+      <c r="C102" s="11"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="15"/>
+      <c r="C103" s="11"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="15"/>
+      <c r="C104" s="11"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="15"/>
+      <c r="C105" s="11"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="15"/>
+      <c r="C106" s="11"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="15"/>
+      <c r="C107" s="11"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="15"/>
+      <c r="C108" s="11"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="15"/>
+      <c r="C109" s="11"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="15"/>
+      <c r="C110" s="11"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="15"/>
+      <c r="C111" s="11"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="15"/>
+      <c r="C112" s="11"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="15"/>
+      <c r="C113" s="11"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="15"/>
+      <c r="C114" s="11"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="15"/>
+      <c r="C115" s="11"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="15"/>
+      <c r="C116" s="11"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="15"/>
+      <c r="C117" s="11"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="15"/>
+      <c r="C118" s="11"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="15"/>
+      <c r="C119" s="11"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="15"/>
+      <c r="C120" s="11"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="15"/>
+      <c r="C121" s="11"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="15"/>
+      <c r="C122" s="11"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="15"/>
+      <c r="C123" s="11"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="15"/>
+      <c r="C124" s="11"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="15"/>
+      <c r="C125" s="11"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="15"/>
+      <c r="C126" s="11"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="15"/>
+      <c r="C127" s="11"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="15"/>
+      <c r="C128" s="11"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="15"/>
+      <c r="C129" s="11"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="15"/>
+      <c r="C130" s="11"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="15"/>
+      <c r="C131" s="11"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="15"/>
+      <c r="C132" s="11"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="15"/>
+      <c r="C133" s="11"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="15"/>
+      <c r="C134" s="11"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="15"/>
+      <c r="C135" s="11"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="15"/>
+      <c r="C136" s="11"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="15"/>
+      <c r="C137" s="11"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="15"/>
+      <c r="C138" s="11"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="15"/>
+      <c r="C139" s="11"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="15"/>
+      <c r="C140" s="11"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="15"/>
+      <c r="C141" s="11"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="15"/>
+      <c r="C142" s="11"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="15"/>
+      <c r="C143" s="11"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="15"/>
+      <c r="C144" s="11"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="15"/>
+      <c r="C145" s="11"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="15"/>
+      <c r="C146" s="11"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="15"/>
+      <c r="C147" s="11"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="15"/>
+      <c r="C148" s="11"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="15"/>
+      <c r="C149" s="11"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="15"/>
+      <c r="C150" s="11"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="15"/>
+      <c r="C151" s="11"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="15"/>
+      <c r="C152" s="11"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="15"/>
+      <c r="C153" s="11"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="15"/>
+      <c r="C154" s="11"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="15"/>
+      <c r="C155" s="11"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="15"/>
+      <c r="C156" s="11"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="15"/>
+      <c r="C157" s="11"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="15"/>
+      <c r="C158" s="11"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="15"/>
+      <c r="C159" s="11"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="15"/>
+      <c r="C160" s="11"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="15"/>
+      <c r="C161" s="11"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="15"/>
+      <c r="C162" s="11"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="15"/>
+      <c r="C163" s="11"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="15"/>
+      <c r="C164" s="11"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="15"/>
+      <c r="C165" s="11"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="15"/>
+      <c r="C166" s="11"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="15"/>
+      <c r="C167" s="11"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="15"/>
+      <c r="C168" s="11"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="15"/>
+      <c r="C169" s="11"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="15"/>
+      <c r="C170" s="11"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="15"/>
+      <c r="C171" s="11"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="15"/>
+      <c r="C172" s="11"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="15"/>
+      <c r="C173" s="11"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="15"/>
+      <c r="C174" s="11"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="15"/>
+      <c r="C175" s="11"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="15"/>
+      <c r="C176" s="11"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="15"/>
+      <c r="C177" s="11"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="15"/>
+      <c r="C178" s="11"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="15"/>
+      <c r="C179" s="11"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="15"/>
+      <c r="C180" s="11"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="15"/>
+      <c r="C181" s="11"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="15"/>
+      <c r="C182" s="11"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="15"/>
+      <c r="C183" s="11"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="15"/>
+      <c r="C184" s="11"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="15"/>
+      <c r="C185" s="11"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="15"/>
+      <c r="C186" s="11"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="15"/>
+      <c r="C187" s="11"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="15"/>
+      <c r="C188" s="11"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="15"/>
+      <c r="C189" s="11"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="15"/>
+      <c r="C190" s="11"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="15"/>
+      <c r="C191" s="11"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="15"/>
+      <c r="C192" s="11"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="15"/>
+      <c r="C193" s="11"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="15"/>
+      <c r="C194" s="11"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="15"/>
+      <c r="C195" s="11"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="15"/>
+      <c r="C196" s="11"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="15"/>
+      <c r="C197" s="11"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="15"/>
+      <c r="C198" s="11"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="15"/>
+      <c r="C199" s="11"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="15"/>
+      <c r="C200" s="11"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="15"/>
+      <c r="C201" s="11"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="15"/>
+      <c r="C202" s="11"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="15"/>
+      <c r="C203" s="11"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="15"/>
+      <c r="C204" s="11"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="15"/>
+      <c r="C205" s="11"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="15"/>
+      <c r="C206" s="11"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="15"/>
+      <c r="C207" s="11"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="15"/>
+      <c r="C208" s="11"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="15"/>
+      <c r="C209" s="11"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="15"/>
+      <c r="C210" s="11"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="15"/>
+      <c r="C211" s="11"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="15"/>
+      <c r="C212" s="11"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="15"/>
+      <c r="C213" s="11"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="15"/>
+      <c r="C214" s="11"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="15"/>
+      <c r="C215" s="11"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="15"/>
+      <c r="C216" s="11"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="15"/>
+      <c r="C217" s="11"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="15"/>
+      <c r="C218" s="11"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="15"/>
+      <c r="C219" s="11"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="15"/>
+      <c r="C220" s="11"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update country model (#137)
* Added regions and subregions in country

* Removed region/subregion
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -193,13 +193,25 @@
   </si>
   <si>
     <t>OOPPP</t>
+  </si>
+  <si>
+    <t>Technical assistance</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>TRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -212,22 +224,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF274180"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -250,65 +253,39 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -545,29 +522,29 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -576,10 +553,10 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -591,10 +568,10 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -606,109 +583,109 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
@@ -723,8 +700,8 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -736,69 +713,69 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -807,9 +784,9 @@
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -818,663 +795,679 @@
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="15"/>
+      <c r="A28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="15"/>
+      <c r="A29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="15"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="15"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="15"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="15"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="15"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="15"/>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="15"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="15"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="15"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="15"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="15"/>
+      <c r="C40" s="11"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="15"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="15"/>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="15"/>
+      <c r="C43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="15"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="15"/>
+      <c r="C45" s="11"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="15"/>
+      <c r="C46" s="11"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="15"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="15"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="15"/>
+      <c r="C49" s="11"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="15"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="15"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="15"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="15"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="15"/>
+      <c r="C54" s="11"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="15"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="15"/>
+      <c r="C56" s="11"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="15"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="15"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="15"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="15"/>
+      <c r="C60" s="11"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="15"/>
+      <c r="C61" s="11"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="15"/>
+      <c r="C62" s="11"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="15"/>
+      <c r="C63" s="11"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="15"/>
+      <c r="C64" s="11"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="15"/>
+      <c r="C65" s="11"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="15"/>
+      <c r="C66" s="11"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="15"/>
+      <c r="C67" s="11"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="15"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="15"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="15"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="15"/>
+      <c r="C71" s="11"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="15"/>
+      <c r="C72" s="11"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="15"/>
+      <c r="C73" s="11"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="15"/>
+      <c r="C74" s="11"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="15"/>
+      <c r="C75" s="11"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="15"/>
+      <c r="C76" s="11"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="15"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="15"/>
+      <c r="C78" s="11"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="15"/>
+      <c r="C79" s="11"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="15"/>
+      <c r="C80" s="11"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="15"/>
+      <c r="C81" s="11"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="15"/>
+      <c r="C82" s="11"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="15"/>
+      <c r="C83" s="11"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="15"/>
+      <c r="C84" s="11"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="15"/>
+      <c r="C85" s="11"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="15"/>
+      <c r="C86" s="11"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="15"/>
+      <c r="C87" s="11"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="15"/>
+      <c r="C88" s="11"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="15"/>
+      <c r="C89" s="11"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="15"/>
+      <c r="C90" s="11"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="15"/>
+      <c r="C91" s="11"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="15"/>
+      <c r="C92" s="11"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="15"/>
+      <c r="C93" s="11"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="15"/>
+      <c r="C94" s="11"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="15"/>
+      <c r="C95" s="11"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="15"/>
+      <c r="C96" s="11"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="15"/>
+      <c r="C97" s="11"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="15"/>
+      <c r="C98" s="11"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="15"/>
+      <c r="C99" s="11"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="15"/>
+      <c r="C100" s="11"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="15"/>
+      <c r="C101" s="11"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="15"/>
+      <c r="C102" s="11"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="15"/>
+      <c r="C103" s="11"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="15"/>
+      <c r="C104" s="11"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="15"/>
+      <c r="C105" s="11"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="15"/>
+      <c r="C106" s="11"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="15"/>
+      <c r="C107" s="11"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="15"/>
+      <c r="C108" s="11"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="15"/>
+      <c r="C109" s="11"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="15"/>
+      <c r="C110" s="11"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="15"/>
+      <c r="C111" s="11"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="15"/>
+      <c r="C112" s="11"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="15"/>
+      <c r="C113" s="11"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="15"/>
+      <c r="C114" s="11"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="15"/>
+      <c r="C115" s="11"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="15"/>
+      <c r="C116" s="11"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="15"/>
+      <c r="C117" s="11"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="15"/>
+      <c r="C118" s="11"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="15"/>
+      <c r="C119" s="11"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="15"/>
+      <c r="C120" s="11"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="15"/>
+      <c r="C121" s="11"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="15"/>
+      <c r="C122" s="11"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="15"/>
+      <c r="C123" s="11"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="15"/>
+      <c r="C124" s="11"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="15"/>
+      <c r="C125" s="11"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="15"/>
+      <c r="C126" s="11"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="15"/>
+      <c r="C127" s="11"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="15"/>
+      <c r="C128" s="11"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="15"/>
+      <c r="C129" s="11"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="15"/>
+      <c r="C130" s="11"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="15"/>
+      <c r="C131" s="11"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="15"/>
+      <c r="C132" s="11"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="15"/>
+      <c r="C133" s="11"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="15"/>
+      <c r="C134" s="11"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="15"/>
+      <c r="C135" s="11"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="15"/>
+      <c r="C136" s="11"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="15"/>
+      <c r="C137" s="11"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="15"/>
+      <c r="C138" s="11"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="15"/>
+      <c r="C139" s="11"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="15"/>
+      <c r="C140" s="11"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="15"/>
+      <c r="C141" s="11"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="15"/>
+      <c r="C142" s="11"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="15"/>
+      <c r="C143" s="11"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="15"/>
+      <c r="C144" s="11"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="15"/>
+      <c r="C145" s="11"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="15"/>
+      <c r="C146" s="11"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="15"/>
+      <c r="C147" s="11"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="15"/>
+      <c r="C148" s="11"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="15"/>
+      <c r="C149" s="11"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="15"/>
+      <c r="C150" s="11"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="15"/>
+      <c r="C151" s="11"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="15"/>
+      <c r="C152" s="11"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="15"/>
+      <c r="C153" s="11"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="15"/>
+      <c r="C154" s="11"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="15"/>
+      <c r="C155" s="11"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="15"/>
+      <c r="C156" s="11"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="15"/>
+      <c r="C157" s="11"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="15"/>
+      <c r="C158" s="11"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="15"/>
+      <c r="C159" s="11"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="15"/>
+      <c r="C160" s="11"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="15"/>
+      <c r="C161" s="11"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="15"/>
+      <c r="C162" s="11"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="15"/>
+      <c r="C163" s="11"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="15"/>
+      <c r="C164" s="11"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="15"/>
+      <c r="C165" s="11"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="15"/>
+      <c r="C166" s="11"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="15"/>
+      <c r="C167" s="11"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="15"/>
+      <c r="C168" s="11"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="15"/>
+      <c r="C169" s="11"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="15"/>
+      <c r="C170" s="11"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="15"/>
+      <c r="C171" s="11"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="15"/>
+      <c r="C172" s="11"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="15"/>
+      <c r="C173" s="11"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="15"/>
+      <c r="C174" s="11"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="15"/>
+      <c r="C175" s="11"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="15"/>
+      <c r="C176" s="11"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="15"/>
+      <c r="C177" s="11"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="15"/>
+      <c r="C178" s="11"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="15"/>
+      <c r="C179" s="11"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="15"/>
+      <c r="C180" s="11"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="15"/>
+      <c r="C181" s="11"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="15"/>
+      <c r="C182" s="11"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="15"/>
+      <c r="C183" s="11"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="15"/>
+      <c r="C184" s="11"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="15"/>
+      <c r="C185" s="11"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="15"/>
+      <c r="C186" s="11"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="15"/>
+      <c r="C187" s="11"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="15"/>
+      <c r="C188" s="11"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="15"/>
+      <c r="C189" s="11"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="15"/>
+      <c r="C190" s="11"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="15"/>
+      <c r="C191" s="11"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="15"/>
+      <c r="C192" s="11"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="15"/>
+      <c r="C193" s="11"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="15"/>
+      <c r="C194" s="11"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="15"/>
+      <c r="C195" s="11"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="15"/>
+      <c r="C196" s="11"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="15"/>
+      <c r="C197" s="11"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="15"/>
+      <c r="C198" s="11"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="15"/>
+      <c r="C199" s="11"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="15"/>
+      <c r="C200" s="11"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="15"/>
+      <c r="C201" s="11"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="15"/>
+      <c r="C202" s="11"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="15"/>
+      <c r="C203" s="11"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="15"/>
+      <c r="C204" s="11"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="15"/>
+      <c r="C205" s="11"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="15"/>
+      <c r="C206" s="11"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="15"/>
+      <c r="C207" s="11"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="15"/>
+      <c r="C208" s="11"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="15"/>
+      <c r="C209" s="11"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="15"/>
+      <c r="C210" s="11"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="15"/>
+      <c r="C211" s="11"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="15"/>
+      <c r="C212" s="11"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="15"/>
+      <c r="C213" s="11"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="15"/>
+      <c r="C214" s="11"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="15"/>
+      <c r="C215" s="11"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="15"/>
+      <c r="C216" s="11"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="15"/>
+      <c r="C217" s="11"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="15"/>
+      <c r="C218" s="11"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="15"/>
+      <c r="C219" s="11"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="15"/>
+      <c r="C220" s="11"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated sector and clusters list
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="d8JdM1G91/1GS+kNXhlyzui+1+JyDp7qXMX0PW1XctA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="GT5WWqYAm3Lp+1Q1KD0iNu6OklzfmB+EQTJXPE5/2D8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -132,18 +132,6 @@
     <t>HPPMP3</t>
   </si>
   <si>
-    <t>Compliance Assistance Programme</t>
-  </si>
-  <si>
-    <t>CAP</t>
-  </si>
-  <si>
-    <t>Core Unit</t>
-  </si>
-  <si>
-    <t>CU</t>
-  </si>
-  <si>
     <t>HFC Individual</t>
   </si>
   <si>
@@ -205,6 +193,9 @@
   </si>
   <si>
     <t>TRA</t>
+  </si>
+  <si>
+    <t>Agency</t>
   </si>
 </sst>
 </file>
@@ -229,8 +220,7 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -273,18 +263,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
@@ -778,697 +763,680 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="9"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C26" s="6"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="11"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="11"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="11"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="11"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="11"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="11"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="11"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="11"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="11"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="11"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="11"/>
+      <c r="C40" s="8"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="11"/>
+      <c r="C41" s="8"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="11"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="11"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="11"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="11"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="11"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="11"/>
+      <c r="C47" s="8"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="11"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="11"/>
+      <c r="C49" s="8"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="11"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="11"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="11"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="11"/>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="11"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="11"/>
+      <c r="C55" s="8"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="11"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="11"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="11"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="11"/>
+      <c r="C59" s="8"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="11"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="11"/>
+      <c r="C61" s="8"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="11"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="11"/>
+      <c r="C63" s="8"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="11"/>
+      <c r="C64" s="8"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="11"/>
+      <c r="C65" s="8"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="11"/>
+      <c r="C66" s="8"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="11"/>
+      <c r="C67" s="8"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="11"/>
+      <c r="C68" s="8"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="11"/>
+      <c r="C69" s="8"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="11"/>
+      <c r="C70" s="8"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="11"/>
+      <c r="C71" s="8"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="11"/>
+      <c r="C72" s="8"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="11"/>
+      <c r="C73" s="8"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="11"/>
+      <c r="C74" s="8"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="11"/>
+      <c r="C75" s="8"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="11"/>
+      <c r="C76" s="8"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="11"/>
+      <c r="C77" s="8"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="11"/>
+      <c r="C78" s="8"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="11"/>
+      <c r="C79" s="8"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="11"/>
+      <c r="C80" s="8"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="11"/>
+      <c r="C81" s="8"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="11"/>
+      <c r="C82" s="8"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="11"/>
+      <c r="C83" s="8"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="11"/>
+      <c r="C84" s="8"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="11"/>
+      <c r="C85" s="8"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="11"/>
+      <c r="C86" s="8"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="11"/>
+      <c r="C87" s="8"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="11"/>
+      <c r="C88" s="8"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="11"/>
+      <c r="C89" s="8"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="11"/>
+      <c r="C90" s="8"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="11"/>
+      <c r="C91" s="8"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="11"/>
+      <c r="C92" s="8"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="11"/>
+      <c r="C93" s="8"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="11"/>
+      <c r="C94" s="8"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="11"/>
+      <c r="C95" s="8"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="11"/>
+      <c r="C96" s="8"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="11"/>
+      <c r="C97" s="8"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="11"/>
+      <c r="C98" s="8"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="11"/>
+      <c r="C99" s="8"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="11"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="11"/>
+      <c r="C101" s="8"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="11"/>
+      <c r="C102" s="8"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="11"/>
+      <c r="C103" s="8"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="11"/>
+      <c r="C104" s="8"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="11"/>
+      <c r="C105" s="8"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="11"/>
+      <c r="C106" s="8"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="11"/>
+      <c r="C107" s="8"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="11"/>
+      <c r="C108" s="8"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="11"/>
+      <c r="C109" s="8"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="11"/>
+      <c r="C110" s="8"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="11"/>
+      <c r="C111" s="8"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="11"/>
+      <c r="C112" s="8"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="11"/>
+      <c r="C113" s="8"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="11"/>
+      <c r="C114" s="8"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="11"/>
+      <c r="C115" s="8"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="11"/>
+      <c r="C116" s="8"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="11"/>
+      <c r="C117" s="8"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="11"/>
+      <c r="C118" s="8"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="11"/>
+      <c r="C119" s="8"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="11"/>
+      <c r="C120" s="8"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="11"/>
+      <c r="C121" s="8"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="11"/>
+      <c r="C122" s="8"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="11"/>
+      <c r="C123" s="8"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="11"/>
+      <c r="C124" s="8"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="11"/>
+      <c r="C125" s="8"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="11"/>
+      <c r="C126" s="8"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="11"/>
+      <c r="C127" s="8"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="11"/>
+      <c r="C128" s="8"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="11"/>
+      <c r="C129" s="8"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="11"/>
+      <c r="C130" s="8"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="11"/>
+      <c r="C131" s="8"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="11"/>
+      <c r="C132" s="8"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="11"/>
+      <c r="C133" s="8"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="11"/>
+      <c r="C134" s="8"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="11"/>
+      <c r="C135" s="8"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="11"/>
+      <c r="C136" s="8"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="11"/>
+      <c r="C137" s="8"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="11"/>
+      <c r="C138" s="8"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="11"/>
+      <c r="C139" s="8"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="11"/>
+      <c r="C140" s="8"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="11"/>
+      <c r="C141" s="8"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="11"/>
+      <c r="C142" s="8"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="11"/>
+      <c r="C143" s="8"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="11"/>
+      <c r="C144" s="8"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="11"/>
+      <c r="C145" s="8"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="11"/>
+      <c r="C146" s="8"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="11"/>
+      <c r="C147" s="8"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="11"/>
+      <c r="C148" s="8"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="11"/>
+      <c r="C149" s="8"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="11"/>
+      <c r="C150" s="8"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="11"/>
+      <c r="C151" s="8"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="11"/>
+      <c r="C152" s="8"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="11"/>
+      <c r="C153" s="8"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="11"/>
+      <c r="C154" s="8"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="11"/>
+      <c r="C155" s="8"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="11"/>
+      <c r="C156" s="8"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="11"/>
+      <c r="C157" s="8"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="11"/>
+      <c r="C158" s="8"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="11"/>
+      <c r="C159" s="8"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="11"/>
+      <c r="C160" s="8"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="11"/>
+      <c r="C161" s="8"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="11"/>
+      <c r="C162" s="8"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="11"/>
+      <c r="C163" s="8"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="11"/>
+      <c r="C164" s="8"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="11"/>
+      <c r="C165" s="8"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="11"/>
+      <c r="C166" s="8"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="11"/>
+      <c r="C167" s="8"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="11"/>
+      <c r="C168" s="8"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="11"/>
+      <c r="C169" s="8"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="11"/>
+      <c r="C170" s="8"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="11"/>
+      <c r="C171" s="8"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="11"/>
+      <c r="C172" s="8"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="11"/>
+      <c r="C173" s="8"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="11"/>
+      <c r="C174" s="8"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="11"/>
+      <c r="C175" s="8"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="11"/>
+      <c r="C176" s="8"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="11"/>
+      <c r="C177" s="8"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="11"/>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="11"/>
+      <c r="C179" s="8"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="11"/>
+      <c r="C180" s="8"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="11"/>
+      <c r="C181" s="8"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="11"/>
+      <c r="C182" s="8"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="11"/>
+      <c r="C183" s="8"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="11"/>
+      <c r="C184" s="8"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="11"/>
+      <c r="C185" s="8"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="11"/>
+      <c r="C186" s="8"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="11"/>
+      <c r="C187" s="8"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="11"/>
+      <c r="C188" s="8"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="11"/>
+      <c r="C189" s="8"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="11"/>
+      <c r="C190" s="8"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="11"/>
+      <c r="C191" s="8"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="11"/>
+      <c r="C192" s="8"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="11"/>
+      <c r="C193" s="8"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="11"/>
+      <c r="C194" s="8"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="11"/>
+      <c r="C195" s="8"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="11"/>
+      <c r="C196" s="8"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="11"/>
+      <c r="C197" s="8"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="11"/>
+      <c r="C198" s="8"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="11"/>
+      <c r="C199" s="8"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="11"/>
+      <c r="C200" s="8"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="11"/>
+      <c r="C201" s="8"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="11"/>
+      <c r="C202" s="8"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="11"/>
+      <c r="C203" s="8"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="11"/>
+      <c r="C204" s="8"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="11"/>
+      <c r="C205" s="8"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="11"/>
+      <c r="C206" s="8"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="11"/>
+      <c r="C207" s="8"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="11"/>
+      <c r="C208" s="8"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="11"/>
+      <c r="C209" s="8"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="11"/>
+      <c r="C210" s="8"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="11"/>
+      <c r="C211" s="8"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="11"/>
+      <c r="C212" s="8"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="11"/>
+      <c r="C213" s="8"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="11"/>
+      <c r="C214" s="8"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="11"/>
+      <c r="C215" s="8"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="11"/>
+      <c r="C216" s="8"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="11"/>
+      <c r="C217" s="8"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="11"/>
-    </row>
-    <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="11"/>
-    </row>
-    <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="11"/>
-    </row>
+      <c r="C218" s="8"/>
+    </row>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
     <row r="223" ht="15.75" customHeight="1"/>
@@ -2247,8 +2215,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted TAS cluster and sector + deleted sector phaseout plan
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="GT5WWqYAm3Lp+1Q1KD0iNu6OklzfmB+EQTJXPE5/2D8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="WyvmzgfdgJ3j+xPfCxGHOG1c63ce2JZVBrcOPo+HbMQ="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -183,12 +183,6 @@
     <t>OOPPP</t>
   </si>
   <si>
-    <t>Technical assistance</t>
-  </si>
-  <si>
-    <t>TAS</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
@@ -196,6 +190,9 @@
   </si>
   <si>
     <t>Agency</t>
+  </si>
+  <si>
+    <t>OOI</t>
   </si>
 </sst>
 </file>
@@ -849,19 +846,17 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C28" s="8"/>
     </row>
@@ -1432,9 +1427,7 @@
     <row r="217" ht="15.75" customHeight="1">
       <c r="C217" s="8"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="8"/>
-    </row>
+    <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
@@ -2214,7 +2207,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update cluster sector list (#144)
* Deleted TAS cluster and sector + deleted sector phaseout plan

* Updated project cluster mapping

* Pylint
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="GT5WWqYAm3Lp+1Q1KD0iNu6OklzfmB+EQTJXPE5/2D8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="WyvmzgfdgJ3j+xPfCxGHOG1c63ce2JZVBrcOPo+HbMQ="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -183,12 +183,6 @@
     <t>OOPPP</t>
   </si>
   <si>
-    <t>Technical assistance</t>
-  </si>
-  <si>
-    <t>TAS</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
@@ -196,6 +190,9 @@
   </si>
   <si>
     <t>Agency</t>
+  </si>
+  <si>
+    <t>OOI</t>
   </si>
 </sst>
 </file>
@@ -849,19 +846,17 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C28" s="8"/>
     </row>
@@ -1432,9 +1427,7 @@
     <row r="217" ht="15.75" customHeight="1">
       <c r="C217" s="8"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="8"/>
-    </row>
+    <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
@@ -2214,7 +2207,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update project cluster mapping
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -192,7 +192,16 @@
     <t>Agency</t>
   </si>
   <si>
+    <t>AGC</t>
+  </si>
+  <si>
     <t>OOI</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>GOV</t>
   </si>
 </sst>
 </file>
@@ -849,18 +858,27 @@
       <c r="A27" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="B27" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Update project cluster mapping (#145)
* Update project cluster mapping

* Pylint
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -192,7 +192,16 @@
     <t>Agency</t>
   </si>
   <si>
+    <t>AGC</t>
+  </si>
+  <si>
     <t>OOI</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>GOV</t>
   </si>
 </sst>
 </file>
@@ -849,18 +858,27 @@
       <c r="A27" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="B27" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updates on project cluster mapping
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -24,10 +24,7 @@
     <t>Acronym</t>
   </si>
   <si>
-    <t>Asscoaited Substance</t>
-  </si>
-  <si>
-    <t>IN BP (Y/N)</t>
+    <t>Category</t>
   </si>
   <si>
     <t>Kigali Implementation Plan Stage 1</t>
@@ -36,10 +33,7 @@
     <t>KIP1</t>
   </si>
   <si>
-    <t>HFC</t>
-  </si>
-  <si>
-    <t>PRP type exists</t>
+    <t>MYA</t>
   </si>
   <si>
     <t>Kigali Implementation Plan Stage 2</t>
@@ -78,9 +72,6 @@
     <t>HPMP1</t>
   </si>
   <si>
-    <t>HCFC</t>
-  </si>
-  <si>
     <t>HCFC phase-out management plan stage 2</t>
   </si>
   <si>
@@ -105,103 +96,109 @@
     <t>EC</t>
   </si>
   <si>
-    <t>Insititutional Strengthening</t>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 1</t>
+  </si>
+  <si>
+    <t>HPPMP1</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 2</t>
+  </si>
+  <si>
+    <t>HPPMP2</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 3</t>
+  </si>
+  <si>
+    <t>HPPMP3</t>
+  </si>
+  <si>
+    <t>HFC Individual</t>
+  </si>
+  <si>
+    <t>HFCIND</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>HCFC Individual</t>
+  </si>
+  <si>
+    <t>HCFCIND</t>
+  </si>
+  <si>
+    <t>Energy Eficiency</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Disposal</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>CFC Individual</t>
+  </si>
+  <si>
+    <t>CFCIND</t>
+  </si>
+  <si>
+    <t>CFC Phase-out Plans</t>
+  </si>
+  <si>
+    <t>CPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Sector Plans</t>
+  </si>
+  <si>
+    <t>OOSP</t>
+  </si>
+  <si>
+    <t>CFC Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>CPPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>OOPPP</t>
+  </si>
+  <si>
+    <t>Other ODS Individual</t>
+  </si>
+  <si>
+    <t>OOI</t>
+  </si>
+  <si>
+    <t>Government Support</t>
+  </si>
+  <si>
+    <t>GOV</t>
+  </si>
+  <si>
+    <t>Agency Programme</t>
+  </si>
+  <si>
+    <t>AGC</t>
+  </si>
+  <si>
+    <t>Country Programme</t>
+  </si>
+  <si>
+    <t>CP</t>
   </si>
   <si>
     <t>INS</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 1</t>
-  </si>
-  <si>
-    <t>HPPMP1</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 2</t>
-  </si>
-  <si>
-    <t>HPPMP2</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 3</t>
-  </si>
-  <si>
-    <t>HPPMP3</t>
-  </si>
-  <si>
-    <t>HFC Individual</t>
-  </si>
-  <si>
-    <t>HFCIND</t>
-  </si>
-  <si>
-    <t>HCFC Individual</t>
-  </si>
-  <si>
-    <t>HCFCIND</t>
-  </si>
-  <si>
-    <t>Energy Eficiency</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>Disposal</t>
-  </si>
-  <si>
-    <t>CFC Individual</t>
-  </si>
-  <si>
-    <t>CFCIND</t>
-  </si>
-  <si>
-    <t>CFC Phase-out Plans</t>
-  </si>
-  <si>
-    <t>CPOP</t>
-  </si>
-  <si>
-    <t>Other ODS Sector Plans</t>
-  </si>
-  <si>
-    <t>OOSP</t>
-  </si>
-  <si>
-    <t>CFC Production Phase out Plans</t>
-  </si>
-  <si>
-    <t>CPPOP</t>
-  </si>
-  <si>
-    <t>Other ODS Production Phase out Plans</t>
-  </si>
-  <si>
-    <t>OOPPP</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>TRA</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>AGC</t>
-  </si>
-  <si>
-    <t>OOI</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>GOV</t>
   </si>
 </sst>
 </file>
@@ -235,18 +232,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFED354"/>
-        <bgColor rgb="FFFED354"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,26 +246,41 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
@@ -496,8 +502,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="49.63"/>
-    <col customWidth="1" min="2" max="2" width="28.75"/>
-    <col customWidth="1" min="3" max="3" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="16.25"/>
+    <col customWidth="1" min="3" max="3" width="11.38"/>
     <col customWidth="1" min="4" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="15.13"/>
     <col customWidth="1" min="6" max="7" width="12.63"/>
@@ -513,9 +519,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -538,912 +542,926 @@
       <c r="X1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="B28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="8"/>
+      <c r="B29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="8"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="8"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="8"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="8"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="8"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="8"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="8"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="8"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="8"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="8"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="8"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="8"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="8"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="8"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="8"/>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="8"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="8"/>
+      <c r="C46" s="13"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="8"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="8"/>
+      <c r="C48" s="13"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="8"/>
+      <c r="C49" s="13"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="8"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="8"/>
+      <c r="C51" s="13"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="8"/>
+      <c r="C52" s="13"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="8"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="8"/>
+      <c r="C54" s="13"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="8"/>
+      <c r="C55" s="13"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="8"/>
+      <c r="C56" s="13"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="8"/>
+      <c r="C57" s="13"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="8"/>
+      <c r="C58" s="13"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="8"/>
+      <c r="C59" s="13"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="8"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="8"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="8"/>
+      <c r="C62" s="13"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="8"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="8"/>
+      <c r="C64" s="13"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="8"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="8"/>
+      <c r="C66" s="13"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="8"/>
+      <c r="C67" s="13"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="8"/>
+      <c r="C68" s="13"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="8"/>
+      <c r="C69" s="13"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="8"/>
+      <c r="C70" s="13"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="8"/>
+      <c r="C71" s="13"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="8"/>
+      <c r="C72" s="13"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="8"/>
+      <c r="C73" s="13"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="8"/>
+      <c r="C74" s="13"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="8"/>
+      <c r="C75" s="13"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="8"/>
+      <c r="C76" s="13"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="8"/>
+      <c r="C77" s="13"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="8"/>
+      <c r="C78" s="13"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="8"/>
+      <c r="C79" s="13"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="8"/>
+      <c r="C80" s="13"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="8"/>
+      <c r="C81" s="13"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="8"/>
+      <c r="C82" s="13"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="8"/>
+      <c r="C83" s="13"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="8"/>
+      <c r="C84" s="13"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="8"/>
+      <c r="C85" s="13"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="8"/>
+      <c r="C86" s="13"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="8"/>
+      <c r="C87" s="13"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="8"/>
+      <c r="C88" s="13"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="8"/>
+      <c r="C89" s="13"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="8"/>
+      <c r="C90" s="13"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="8"/>
+      <c r="C91" s="13"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="8"/>
+      <c r="C92" s="13"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="8"/>
+      <c r="C93" s="13"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="8"/>
+      <c r="C94" s="13"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="8"/>
+      <c r="C95" s="13"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="8"/>
+      <c r="C96" s="13"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="8"/>
+      <c r="C97" s="13"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="8"/>
+      <c r="C98" s="13"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="8"/>
+      <c r="C99" s="13"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="8"/>
+      <c r="C100" s="13"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="8"/>
+      <c r="C101" s="13"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="8"/>
+      <c r="C102" s="13"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="8"/>
+      <c r="C103" s="13"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="8"/>
+      <c r="C104" s="13"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="8"/>
+      <c r="C105" s="13"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="8"/>
+      <c r="C106" s="13"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="8"/>
+      <c r="C107" s="13"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="8"/>
+      <c r="C108" s="13"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="8"/>
+      <c r="C109" s="13"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="8"/>
+      <c r="C110" s="13"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="8"/>
+      <c r="C111" s="13"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="8"/>
+      <c r="C112" s="13"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="8"/>
+      <c r="C113" s="13"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="8"/>
+      <c r="C114" s="13"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="8"/>
+      <c r="C115" s="13"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="8"/>
+      <c r="C116" s="13"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="8"/>
+      <c r="C117" s="13"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="8"/>
+      <c r="C118" s="13"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="8"/>
+      <c r="C119" s="13"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="8"/>
+      <c r="C120" s="13"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="8"/>
+      <c r="C121" s="13"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="8"/>
+      <c r="C122" s="13"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="8"/>
+      <c r="C123" s="13"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="8"/>
+      <c r="C124" s="13"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="8"/>
+      <c r="C125" s="13"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="8"/>
+      <c r="C126" s="13"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="8"/>
+      <c r="C127" s="13"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="8"/>
+      <c r="C128" s="13"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="8"/>
+      <c r="C129" s="13"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="8"/>
+      <c r="C130" s="13"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="8"/>
+      <c r="C131" s="13"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="8"/>
+      <c r="C132" s="13"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="8"/>
+      <c r="C133" s="13"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="8"/>
+      <c r="C134" s="13"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="8"/>
+      <c r="C135" s="13"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="8"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="8"/>
+      <c r="C137" s="13"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="8"/>
+      <c r="C138" s="13"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="8"/>
+      <c r="C139" s="13"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="8"/>
+      <c r="C140" s="13"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="8"/>
+      <c r="C141" s="13"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="8"/>
+      <c r="C142" s="13"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="8"/>
+      <c r="C143" s="13"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="8"/>
+      <c r="C144" s="13"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="8"/>
+      <c r="C145" s="13"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="8"/>
+      <c r="C146" s="13"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="8"/>
+      <c r="C147" s="13"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="8"/>
+      <c r="C148" s="13"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="8"/>
+      <c r="C149" s="13"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="8"/>
+      <c r="C150" s="13"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="8"/>
+      <c r="C151" s="13"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="8"/>
+      <c r="C152" s="13"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="8"/>
+      <c r="C153" s="13"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="8"/>
+      <c r="C154" s="13"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="8"/>
+      <c r="C155" s="13"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="8"/>
+      <c r="C156" s="13"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="8"/>
+      <c r="C157" s="13"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="8"/>
+      <c r="C158" s="13"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="8"/>
+      <c r="C159" s="13"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="8"/>
+      <c r="C160" s="13"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="8"/>
+      <c r="C161" s="13"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="8"/>
+      <c r="C162" s="13"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="8"/>
+      <c r="C163" s="13"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="8"/>
+      <c r="C164" s="13"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="8"/>
+      <c r="C165" s="13"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="8"/>
+      <c r="C166" s="13"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="8"/>
+      <c r="C167" s="13"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="8"/>
+      <c r="C168" s="13"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="8"/>
+      <c r="C169" s="13"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="8"/>
+      <c r="C170" s="13"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="8"/>
+      <c r="C171" s="13"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="8"/>
+      <c r="C172" s="13"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="8"/>
+      <c r="C173" s="13"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="8"/>
+      <c r="C174" s="13"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="8"/>
+      <c r="C175" s="13"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="8"/>
+      <c r="C176" s="13"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="8"/>
+      <c r="C177" s="13"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="8"/>
+      <c r="C178" s="13"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="8"/>
+      <c r="C179" s="13"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="8"/>
+      <c r="C180" s="13"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="8"/>
+      <c r="C181" s="13"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="8"/>
+      <c r="C182" s="13"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="8"/>
+      <c r="C183" s="13"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="8"/>
+      <c r="C184" s="13"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="8"/>
+      <c r="C185" s="13"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="8"/>
+      <c r="C186" s="13"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="8"/>
+      <c r="C187" s="13"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="8"/>
+      <c r="C188" s="13"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="8"/>
+      <c r="C189" s="13"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="8"/>
+      <c r="C190" s="13"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="8"/>
+      <c r="C191" s="13"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="8"/>
+      <c r="C192" s="13"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="8"/>
+      <c r="C193" s="13"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="8"/>
+      <c r="C194" s="13"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="8"/>
+      <c r="C195" s="13"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="8"/>
+      <c r="C196" s="13"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="8"/>
+      <c r="C197" s="13"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="8"/>
+      <c r="C198" s="13"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="8"/>
+      <c r="C199" s="13"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="8"/>
+      <c r="C200" s="13"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="8"/>
+      <c r="C201" s="13"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="8"/>
+      <c r="C202" s="13"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="8"/>
+      <c r="C203" s="13"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="8"/>
+      <c r="C204" s="13"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="8"/>
+      <c r="C205" s="13"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="8"/>
+      <c r="C206" s="13"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="8"/>
+      <c r="C207" s="13"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="8"/>
+      <c r="C208" s="13"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="8"/>
+      <c r="C209" s="13"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="8"/>
+      <c r="C210" s="13"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="8"/>
+      <c r="C211" s="13"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="8"/>
+      <c r="C212" s="13"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="8"/>
+      <c r="C213" s="13"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="8"/>
+      <c r="C214" s="13"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="8"/>
+      <c r="C215" s="13"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="8"/>
+      <c r="C216" s="13"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="8"/>
+      <c r="C217" s="13"/>
     </row>
     <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updates on project cluster mapping (#146)
* Updates on project cluster mapping

* Fixed tests
</commit_message>
<xml_diff>
--- a/core/import_data/resources/project_clusters.xlsx
+++ b/core/import_data/resources/project_clusters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -24,10 +24,7 @@
     <t>Acronym</t>
   </si>
   <si>
-    <t>Asscoaited Substance</t>
-  </si>
-  <si>
-    <t>IN BP (Y/N)</t>
+    <t>Category</t>
   </si>
   <si>
     <t>Kigali Implementation Plan Stage 1</t>
@@ -36,10 +33,7 @@
     <t>KIP1</t>
   </si>
   <si>
-    <t>HFC</t>
-  </si>
-  <si>
-    <t>PRP type exists</t>
+    <t>MYA</t>
   </si>
   <si>
     <t>Kigali Implementation Plan Stage 2</t>
@@ -78,9 +72,6 @@
     <t>HPMP1</t>
   </si>
   <si>
-    <t>HCFC</t>
-  </si>
-  <si>
     <t>HCFC phase-out management plan stage 2</t>
   </si>
   <si>
@@ -105,103 +96,109 @@
     <t>EC</t>
   </si>
   <si>
-    <t>Insititutional Strengthening</t>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 1</t>
+  </si>
+  <si>
+    <t>HPPMP1</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 2</t>
+  </si>
+  <si>
+    <t>HPPMP2</t>
+  </si>
+  <si>
+    <t>HCFC production phase-out management plan stage 3</t>
+  </si>
+  <si>
+    <t>HPPMP3</t>
+  </si>
+  <si>
+    <t>HFC Individual</t>
+  </si>
+  <si>
+    <t>HFCIND</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>HCFC Individual</t>
+  </si>
+  <si>
+    <t>HCFCIND</t>
+  </si>
+  <si>
+    <t>Energy Eficiency</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Disposal</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>CFC Individual</t>
+  </si>
+  <si>
+    <t>CFCIND</t>
+  </si>
+  <si>
+    <t>CFC Phase-out Plans</t>
+  </si>
+  <si>
+    <t>CPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Sector Plans</t>
+  </si>
+  <si>
+    <t>OOSP</t>
+  </si>
+  <si>
+    <t>CFC Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>CPPOP</t>
+  </si>
+  <si>
+    <t>Other ODS Production Phase out Plans</t>
+  </si>
+  <si>
+    <t>OOPPP</t>
+  </si>
+  <si>
+    <t>Other ODS Individual</t>
+  </si>
+  <si>
+    <t>OOI</t>
+  </si>
+  <si>
+    <t>Government Support</t>
+  </si>
+  <si>
+    <t>GOV</t>
+  </si>
+  <si>
+    <t>Agency Programme</t>
+  </si>
+  <si>
+    <t>AGC</t>
+  </si>
+  <si>
+    <t>Country Programme</t>
+  </si>
+  <si>
+    <t>CP</t>
   </si>
   <si>
     <t>INS</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 1</t>
-  </si>
-  <si>
-    <t>HPPMP1</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 2</t>
-  </si>
-  <si>
-    <t>HPPMP2</t>
-  </si>
-  <si>
-    <t>HCFC production phase-out management plan stage 3</t>
-  </si>
-  <si>
-    <t>HPPMP3</t>
-  </si>
-  <si>
-    <t>HFC Individual</t>
-  </si>
-  <si>
-    <t>HFCIND</t>
-  </si>
-  <si>
-    <t>HCFC Individual</t>
-  </si>
-  <si>
-    <t>HCFCIND</t>
-  </si>
-  <si>
-    <t>Energy Eficiency</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>Disposal</t>
-  </si>
-  <si>
-    <t>CFC Individual</t>
-  </si>
-  <si>
-    <t>CFCIND</t>
-  </si>
-  <si>
-    <t>CFC Phase-out Plans</t>
-  </si>
-  <si>
-    <t>CPOP</t>
-  </si>
-  <si>
-    <t>Other ODS Sector Plans</t>
-  </si>
-  <si>
-    <t>OOSP</t>
-  </si>
-  <si>
-    <t>CFC Production Phase out Plans</t>
-  </si>
-  <si>
-    <t>CPPOP</t>
-  </si>
-  <si>
-    <t>Other ODS Production Phase out Plans</t>
-  </si>
-  <si>
-    <t>OOPPP</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>TRA</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>AGC</t>
-  </si>
-  <si>
-    <t>OOI</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>GOV</t>
   </si>
 </sst>
 </file>
@@ -235,18 +232,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFED354"/>
-        <bgColor rgb="FFFED354"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,26 +246,41 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
@@ -496,8 +502,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="49.63"/>
-    <col customWidth="1" min="2" max="2" width="28.75"/>
-    <col customWidth="1" min="3" max="3" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="16.25"/>
+    <col customWidth="1" min="3" max="3" width="11.38"/>
     <col customWidth="1" min="4" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="15.13"/>
     <col customWidth="1" min="6" max="7" width="12.63"/>
@@ -513,9 +519,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -538,912 +542,926 @@
       <c r="X1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="B28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="8"/>
+      <c r="B29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="8"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="8"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="8"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="8"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="8"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="8"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="8"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="8"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="8"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="8"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="8"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="8"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="8"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="8"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="8"/>
+      <c r="C44" s="13"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="8"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="8"/>
+      <c r="C46" s="13"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="8"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="8"/>
+      <c r="C48" s="13"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="8"/>
+      <c r="C49" s="13"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="8"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="8"/>
+      <c r="C51" s="13"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="8"/>
+      <c r="C52" s="13"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="8"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="8"/>
+      <c r="C54" s="13"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="8"/>
+      <c r="C55" s="13"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="8"/>
+      <c r="C56" s="13"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="8"/>
+      <c r="C57" s="13"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="8"/>
+      <c r="C58" s="13"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="8"/>
+      <c r="C59" s="13"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="8"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="8"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="8"/>
+      <c r="C62" s="13"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="8"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="8"/>
+      <c r="C64" s="13"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="8"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="8"/>
+      <c r="C66" s="13"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="8"/>
+      <c r="C67" s="13"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="8"/>
+      <c r="C68" s="13"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="8"/>
+      <c r="C69" s="13"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="8"/>
+      <c r="C70" s="13"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="8"/>
+      <c r="C71" s="13"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="8"/>
+      <c r="C72" s="13"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="8"/>
+      <c r="C73" s="13"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="8"/>
+      <c r="C74" s="13"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="8"/>
+      <c r="C75" s="13"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="8"/>
+      <c r="C76" s="13"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="8"/>
+      <c r="C77" s="13"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="8"/>
+      <c r="C78" s="13"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="8"/>
+      <c r="C79" s="13"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="8"/>
+      <c r="C80" s="13"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="8"/>
+      <c r="C81" s="13"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="8"/>
+      <c r="C82" s="13"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="8"/>
+      <c r="C83" s="13"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="8"/>
+      <c r="C84" s="13"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="8"/>
+      <c r="C85" s="13"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="8"/>
+      <c r="C86" s="13"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="8"/>
+      <c r="C87" s="13"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="8"/>
+      <c r="C88" s="13"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="8"/>
+      <c r="C89" s="13"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="8"/>
+      <c r="C90" s="13"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="8"/>
+      <c r="C91" s="13"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="8"/>
+      <c r="C92" s="13"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="8"/>
+      <c r="C93" s="13"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="8"/>
+      <c r="C94" s="13"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="8"/>
+      <c r="C95" s="13"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="8"/>
+      <c r="C96" s="13"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="8"/>
+      <c r="C97" s="13"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="8"/>
+      <c r="C98" s="13"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="8"/>
+      <c r="C99" s="13"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="8"/>
+      <c r="C100" s="13"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="8"/>
+      <c r="C101" s="13"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="8"/>
+      <c r="C102" s="13"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="8"/>
+      <c r="C103" s="13"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="8"/>
+      <c r="C104" s="13"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="8"/>
+      <c r="C105" s="13"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="8"/>
+      <c r="C106" s="13"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="8"/>
+      <c r="C107" s="13"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="8"/>
+      <c r="C108" s="13"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="8"/>
+      <c r="C109" s="13"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="8"/>
+      <c r="C110" s="13"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="8"/>
+      <c r="C111" s="13"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="8"/>
+      <c r="C112" s="13"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="8"/>
+      <c r="C113" s="13"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="8"/>
+      <c r="C114" s="13"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="8"/>
+      <c r="C115" s="13"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="8"/>
+      <c r="C116" s="13"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="8"/>
+      <c r="C117" s="13"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="8"/>
+      <c r="C118" s="13"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="8"/>
+      <c r="C119" s="13"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="8"/>
+      <c r="C120" s="13"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="8"/>
+      <c r="C121" s="13"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="8"/>
+      <c r="C122" s="13"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="8"/>
+      <c r="C123" s="13"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="8"/>
+      <c r="C124" s="13"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="8"/>
+      <c r="C125" s="13"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="8"/>
+      <c r="C126" s="13"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="8"/>
+      <c r="C127" s="13"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="8"/>
+      <c r="C128" s="13"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="8"/>
+      <c r="C129" s="13"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="8"/>
+      <c r="C130" s="13"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="8"/>
+      <c r="C131" s="13"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="8"/>
+      <c r="C132" s="13"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="8"/>
+      <c r="C133" s="13"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="8"/>
+      <c r="C134" s="13"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="8"/>
+      <c r="C135" s="13"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="8"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="8"/>
+      <c r="C137" s="13"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="8"/>
+      <c r="C138" s="13"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="8"/>
+      <c r="C139" s="13"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="8"/>
+      <c r="C140" s="13"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="8"/>
+      <c r="C141" s="13"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="8"/>
+      <c r="C142" s="13"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="8"/>
+      <c r="C143" s="13"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="8"/>
+      <c r="C144" s="13"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="8"/>
+      <c r="C145" s="13"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="8"/>
+      <c r="C146" s="13"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="8"/>
+      <c r="C147" s="13"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="8"/>
+      <c r="C148" s="13"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="8"/>
+      <c r="C149" s="13"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="8"/>
+      <c r="C150" s="13"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="8"/>
+      <c r="C151" s="13"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="8"/>
+      <c r="C152" s="13"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="8"/>
+      <c r="C153" s="13"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="8"/>
+      <c r="C154" s="13"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="8"/>
+      <c r="C155" s="13"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="8"/>
+      <c r="C156" s="13"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="8"/>
+      <c r="C157" s="13"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="8"/>
+      <c r="C158" s="13"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="8"/>
+      <c r="C159" s="13"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="8"/>
+      <c r="C160" s="13"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="8"/>
+      <c r="C161" s="13"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="8"/>
+      <c r="C162" s="13"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="8"/>
+      <c r="C163" s="13"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="8"/>
+      <c r="C164" s="13"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="8"/>
+      <c r="C165" s="13"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="8"/>
+      <c r="C166" s="13"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="8"/>
+      <c r="C167" s="13"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="8"/>
+      <c r="C168" s="13"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="8"/>
+      <c r="C169" s="13"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="8"/>
+      <c r="C170" s="13"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="8"/>
+      <c r="C171" s="13"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="8"/>
+      <c r="C172" s="13"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="8"/>
+      <c r="C173" s="13"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="8"/>
+      <c r="C174" s="13"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="8"/>
+      <c r="C175" s="13"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="8"/>
+      <c r="C176" s="13"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="8"/>
+      <c r="C177" s="13"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="8"/>
+      <c r="C178" s="13"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="8"/>
+      <c r="C179" s="13"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="8"/>
+      <c r="C180" s="13"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="8"/>
+      <c r="C181" s="13"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="8"/>
+      <c r="C182" s="13"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="8"/>
+      <c r="C183" s="13"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="8"/>
+      <c r="C184" s="13"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="8"/>
+      <c r="C185" s="13"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="8"/>
+      <c r="C186" s="13"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="8"/>
+      <c r="C187" s="13"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="8"/>
+      <c r="C188" s="13"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="8"/>
+      <c r="C189" s="13"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="8"/>
+      <c r="C190" s="13"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="8"/>
+      <c r="C191" s="13"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="8"/>
+      <c r="C192" s="13"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="8"/>
+      <c r="C193" s="13"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="8"/>
+      <c r="C194" s="13"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="8"/>
+      <c r="C195" s="13"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="8"/>
+      <c r="C196" s="13"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="8"/>
+      <c r="C197" s="13"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="8"/>
+      <c r="C198" s="13"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="8"/>
+      <c r="C199" s="13"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="8"/>
+      <c r="C200" s="13"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="8"/>
+      <c r="C201" s="13"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="8"/>
+      <c r="C202" s="13"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="8"/>
+      <c r="C203" s="13"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="8"/>
+      <c r="C204" s="13"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="8"/>
+      <c r="C205" s="13"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="8"/>
+      <c r="C206" s="13"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="8"/>
+      <c r="C207" s="13"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="8"/>
+      <c r="C208" s="13"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="8"/>
+      <c r="C209" s="13"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="8"/>
+      <c r="C210" s="13"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="8"/>
+      <c r="C211" s="13"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="8"/>
+      <c r="C212" s="13"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="8"/>
+      <c r="C213" s="13"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="8"/>
+      <c r="C214" s="13"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="8"/>
+      <c r="C215" s="13"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="8"/>
+      <c r="C216" s="13"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="8"/>
+      <c r="C217" s="13"/>
     </row>
     <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>

</xml_diff>